<commit_message>
feat update row 2000 20001
</commit_message>
<xml_diff>
--- a/testdata/mock_item_data.xlsx
+++ b/testdata/mock_item_data.xlsx
@@ -12236,13 +12236,13 @@
     <t>desc-1999</t>
   </si>
   <si>
-    <t>item-2000</t>
+    <t>item-2020</t>
   </si>
   <si>
     <t>desc-2000</t>
   </si>
   <si>
-    <t>item-2001</t>
+    <t>item-2021</t>
   </si>
   <si>
     <t>desc-2020</t>
@@ -13217,7 +13217,7 @@
   <dimension ref="A1:N2002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1965" workbookViewId="0">
-      <selection activeCell="H2005" sqref="H2005"/>
+      <selection activeCell="B2002" sqref="B2002"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
update row 2000 again
</commit_message>
<xml_diff>
--- a/testdata/mock_item_data.xlsx
+++ b/testdata/mock_item_data.xlsx
@@ -12230,7 +12230,7 @@
     <t>desc-1999</t>
   </si>
   <si>
-    <t>item-2030</t>
+    <t>item-2040</t>
   </si>
   <si>
     <t>desc-2000</t>
@@ -13204,7 +13204,7 @@
   <dimension ref="A1:N2001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1965" workbookViewId="0">
-      <selection activeCell="B2000" sqref="B2000"/>
+      <selection activeCell="D2000" sqref="D2000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>